<commit_message>
finally got a working solution for minavg but needed help
</commit_message>
<xml_diff>
--- a/CodePlayground/Workings.xlsx
+++ b/CodePlayground/Workings.xlsx
@@ -375,15 +375,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:L14"/>
+  <dimension ref="B1:Q14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>2</v>
       </c>
@@ -393,20 +393,20 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>0</v>
       </c>
-      <c r="G1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I1" t="s">
-        <v>4</v>
+      <c r="H1" t="s">
+        <v>1</v>
       </c>
       <c r="J1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2">
         <v>1</v>
       </c>
@@ -416,28 +416,34 @@
       <c r="D2">
         <v>4</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <f>AVERAGE(D2)</f>
         <v>4</v>
       </c>
-      <c r="G2">
-        <f>F2/B2</f>
-        <v>4</v>
-      </c>
-      <c r="I2">
-        <f t="shared" ref="I2:I6" si="0">I3+D2</f>
+      <c r="H2">
+        <f>G2/B2</f>
+        <v>4</v>
+      </c>
+      <c r="J2">
+        <f t="shared" ref="J2:J6" si="0">J3+D2</f>
         <v>27</v>
       </c>
-      <c r="J2">
-        <f t="shared" ref="J2:J7" si="1">I2/C2</f>
+      <c r="K2">
+        <f t="shared" ref="K2:K7" si="1">J2/C2</f>
         <v>3.8571428571428572</v>
       </c>
-      <c r="L2">
-        <f>SUM(G2,J2)</f>
+      <c r="M2">
+        <f>SUM(H2,K2)</f>
         <v>7.8571428571428577</v>
       </c>
-    </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>2</v>
       </c>
@@ -447,28 +453,42 @@
       <c r="D3">
         <v>2</v>
       </c>
+      <c r="E3">
+        <f>D3-D2</f>
+        <v>-2</v>
+      </c>
       <c r="F3">
-        <f>F2+D3</f>
+        <f>E3+F2</f>
+        <v>-2</v>
+      </c>
+      <c r="G3">
+        <f>G2+D3</f>
         <v>6</v>
       </c>
-      <c r="G3">
-        <f>F3/B3</f>
-        <v>3</v>
-      </c>
-      <c r="I3">
+      <c r="H3">
+        <f>G3/B3</f>
+        <v>3</v>
+      </c>
+      <c r="J3">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <f t="shared" si="1"/>
         <v>3.8333333333333335</v>
       </c>
-      <c r="L3">
-        <f t="shared" ref="L3:L8" si="2">SUM(G3,J3)</f>
+      <c r="M3">
+        <f t="shared" ref="M3:M8" si="2">SUM(H3,K3)</f>
         <v>6.8333333333333339</v>
       </c>
-    </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="P3">
+        <v>15</v>
+      </c>
+      <c r="Q3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>3</v>
       </c>
@@ -478,28 +498,42 @@
       <c r="D4">
         <v>2</v>
       </c>
+      <c r="E4">
+        <f t="shared" ref="E4:E8" si="3">D4-D3</f>
+        <v>0</v>
+      </c>
       <c r="F4">
-        <f>F3+D4</f>
+        <f t="shared" ref="F4:F8" si="4">E4+F3</f>
+        <v>-2</v>
+      </c>
+      <c r="G4">
+        <f>G3+D4</f>
         <v>8</v>
       </c>
-      <c r="G4">
-        <f t="shared" ref="G4:G8" si="3">F4/B4</f>
+      <c r="H4">
+        <f t="shared" ref="H4:H8" si="5">G4/B4</f>
         <v>2.6666666666666665</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <f t="shared" si="1"/>
         <v>4.2</v>
       </c>
-      <c r="L4">
+      <c r="M4">
         <f t="shared" si="2"/>
         <v>6.8666666666666671</v>
       </c>
-    </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="P4">
+        <v>5</v>
+      </c>
+      <c r="Q4">
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="5" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>4</v>
       </c>
@@ -509,28 +543,36 @@
       <c r="D5">
         <v>5</v>
       </c>
+      <c r="E5">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
       <c r="F5">
-        <f t="shared" ref="F5:F8" si="4">F4+D5</f>
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <f t="shared" ref="G5:G8" si="6">G4+D5</f>
         <v>13</v>
       </c>
-      <c r="G5">
-        <f t="shared" si="3"/>
+      <c r="H5">
+        <f t="shared" si="5"/>
         <v>3.25</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <f t="shared" si="1"/>
         <v>4.75</v>
       </c>
-      <c r="L5">
+      <c r="M5">
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>5</v>
       </c>
@@ -540,28 +582,36 @@
       <c r="D6">
         <v>1</v>
       </c>
+      <c r="E6">
+        <f t="shared" si="3"/>
+        <v>-4</v>
+      </c>
       <c r="F6">
         <f t="shared" si="4"/>
+        <v>-3</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="6"/>
         <v>14</v>
       </c>
-      <c r="G6">
-        <f t="shared" si="3"/>
+      <c r="H6">
+        <f t="shared" si="5"/>
         <v>2.8</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <f t="shared" si="1"/>
         <v>4.666666666666667</v>
       </c>
-      <c r="L6">
+      <c r="M6">
         <f t="shared" si="2"/>
         <v>7.4666666666666668</v>
       </c>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>6</v>
       </c>
@@ -571,28 +621,36 @@
       <c r="D7">
         <v>5</v>
       </c>
+      <c r="E7">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
       <c r="F7">
         <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="6"/>
         <v>19</v>
       </c>
-      <c r="G7">
-        <f t="shared" si="3"/>
+      <c r="H7">
+        <f t="shared" si="5"/>
         <v>3.1666666666666665</v>
       </c>
-      <c r="I7">
-        <f>I8+D7</f>
+      <c r="J7">
+        <f>J8+D7</f>
         <v>13</v>
       </c>
-      <c r="J7">
+      <c r="K7">
         <f t="shared" si="1"/>
         <v>6.5</v>
       </c>
-      <c r="L7">
+      <c r="M7">
         <f t="shared" si="2"/>
         <v>9.6666666666666661</v>
       </c>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>7</v>
       </c>
@@ -602,28 +660,36 @@
       <c r="D8">
         <v>8</v>
       </c>
+      <c r="E8">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
       <c r="F8">
         <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="6"/>
         <v>27</v>
       </c>
-      <c r="G8">
-        <f t="shared" si="3"/>
+      <c r="H8">
+        <f t="shared" si="5"/>
         <v>3.8571428571428572</v>
       </c>
-      <c r="I8">
+      <c r="J8">
         <f>D8</f>
         <v>8</v>
       </c>
-      <c r="J8">
-        <f>I8/C8</f>
+      <c r="K8">
+        <f>J8/C8</f>
         <v>8</v>
       </c>
-      <c r="L8">
+      <c r="M8">
         <f t="shared" si="2"/>
         <v>11.857142857142858</v>
       </c>
     </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>2</v>
       </c>
@@ -633,20 +699,20 @@
       <c r="D11" t="s">
         <v>3</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>0</v>
       </c>
-      <c r="G11" t="s">
-        <v>1</v>
-      </c>
-      <c r="I11" t="s">
-        <v>4</v>
+      <c r="H11" t="s">
+        <v>1</v>
       </c>
       <c r="J11" t="s">
+        <v>4</v>
+      </c>
+      <c r="K11" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>1</v>
       </c>
@@ -656,28 +722,28 @@
       <c r="D12">
         <v>1</v>
       </c>
-      <c r="F12">
+      <c r="G12">
         <f>AVERAGE(D12)</f>
         <v>1</v>
       </c>
-      <c r="G12">
-        <f>F12/B12</f>
-        <v>1</v>
-      </c>
-      <c r="I12">
-        <f t="shared" ref="I12:I16" si="5">I13+D12</f>
+      <c r="H12">
+        <f>G12/B12</f>
+        <v>1</v>
+      </c>
+      <c r="J12">
+        <f t="shared" ref="J12:J13" si="7">J13+D12</f>
         <v>6</v>
       </c>
-      <c r="J12">
-        <f t="shared" ref="J12:J17" si="6">I12/C12</f>
+      <c r="K12">
+        <f t="shared" ref="K12:K13" si="8">J12/C12</f>
         <v>6</v>
       </c>
-      <c r="L12">
-        <f>SUM(G12,J12)</f>
+      <c r="M12">
+        <f>SUM(H12,K12)</f>
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>2</v>
       </c>
@@ -687,28 +753,28 @@
       <c r="D13">
         <v>2</v>
       </c>
-      <c r="F13">
-        <f>F12+D13</f>
-        <v>3</v>
-      </c>
       <c r="G13">
-        <f>F13/B13</f>
+        <f>G12+D13</f>
+        <v>3</v>
+      </c>
+      <c r="H13">
+        <f>G13/B13</f>
         <v>1.5</v>
       </c>
-      <c r="I13">
-        <f t="shared" si="5"/>
+      <c r="J13">
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
-      <c r="J13">
-        <f t="shared" si="6"/>
+      <c r="K13">
+        <f t="shared" si="8"/>
         <v>2.5</v>
       </c>
-      <c r="L13">
-        <f t="shared" ref="L13:L18" si="7">SUM(G13,J13)</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M13">
+        <f t="shared" ref="M13:M14" si="9">SUM(H13,K13)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B14">
         <v>3</v>
       </c>
@@ -718,24 +784,24 @@
       <c r="D14">
         <v>3</v>
       </c>
-      <c r="F14">
-        <f>F13+D14</f>
+      <c r="G14">
+        <f>G13+D14</f>
         <v>6</v>
       </c>
-      <c r="G14">
-        <f>F14/B14</f>
-        <v>2</v>
-      </c>
-      <c r="I14">
-        <f t="shared" ref="I14" si="8">I15+D14</f>
-        <v>3</v>
+      <c r="H14">
+        <f>G14/B14</f>
+        <v>2</v>
       </c>
       <c r="J14">
-        <f t="shared" ref="J14" si="9">I14/C14</f>
-        <v>1</v>
-      </c>
-      <c r="L14">
-        <f t="shared" si="7"/>
+        <f t="shared" ref="J14" si="10">J15+D14</f>
+        <v>3</v>
+      </c>
+      <c r="K14">
+        <f t="shared" ref="K14" si="11">J14/C14</f>
+        <v>1</v>
+      </c>
+      <c r="M14">
+        <f t="shared" si="9"/>
         <v>3</v>
       </c>
     </row>

</xml_diff>